<commit_message>
PIN-847: fixed tests to work with short version of locations
</commit_message>
<xml_diff>
--- a/tests/NewApiBundle/Resources/CorrectImport.xlsx
+++ b/tests/NewApiBundle/Resources/CorrectImport.xlsx
@@ -416,7 +416,7 @@
     <t xml:space="preserve">kirxwdeumw</t>
   </si>
   <si>
-    <t xml:space="preserve">Battambang</t>
+    <t xml:space="preserve">Banteay Meanchey</t>
   </si>
   <si>
     <t xml:space="preserve">Edwin</t>
@@ -613,8 +613,8 @@
   </sheetPr>
   <dimension ref="A1:BG10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AL7" activeCellId="0" sqref="AL7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>